<commit_message>
upgraded the program for specific cases
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,14 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/v.syroiezhin/Desktop/github/xlsx-data-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9056D2EA-B9AE-FC41-B8F7-04EB4D52E5C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E65EC1-DABC-B94D-BB5E-85F915237DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{34081E2E-10CE-E447-A8CF-169C75E9375B}"/>
   </bookViews>
   <sheets>
     <sheet name="FIRST" sheetId="1" r:id="rId1"/>
-    <sheet name="SECOND" sheetId="2" r:id="rId2"/>
-    <sheet name="THIRD" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>А</t>
   </si>
@@ -410,7 +408,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -451,100 +449,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC12FABC-3FDA-354F-AFD5-BA7FC55D0B6D}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FEFC92B-9CD4-1349-AD84-DE550A38B3AC}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>